<commit_message>
New Tcs and screenshot functionality
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshirodkar/Desktop/Git/Amazon_Demo_Test/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AFFF0F-86F7-0B4D-909E-A96A69A59C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2950F1-2729-BA4B-BC9B-1396EA96EC57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{D261FC6C-52F6-F944-88CE-5A09535C6322}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
-  <si>
-    <t>AmazonLogin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>AmazonSearchItem</t>
   </si>
@@ -67,6 +64,15 @@
   </si>
   <si>
     <t>payment mode</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>AmazonCorrectLogin</t>
+  </si>
+  <si>
+    <t>AmazonIncorrectLogin</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6317A1-9BDC-344A-AEC3-6C87339C1434}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,70 +440,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>7020214690</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>7020214690</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1">
         <v>7020214690</v>
       </c>
       <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7020214690</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>